<commit_message>
correcion de un link
</commit_message>
<xml_diff>
--- a/1-sesion/Thesaurus.xlsx
+++ b/1-sesion/Thesaurus.xlsx
@@ -353,9 +353,6 @@
     <t>"patrones de diseños"</t>
   </si>
   <si>
-    <t>https://d1wqtxts1xzle7.cloudfront.net/60132311/Introduccion-a-los-patrones-de-diseno20190727-56910-x3jn57-libre.pdf?1564251816=&amp;response-content-disposition=inline%3B+filename%3DIntroduccion_a_los_patrones_de_diseno.pdf&amp;Expires=1731430720&amp;Signature=AOBStQ-XLqZ0197XWeU205Jj71Sx-foxddYAWTGMq3ms82sLcv4pOfa2Qxr6u51zdTwDb-sAiAj-j~c4nXOM7Xapd8jqPs-twpYdNFuj2ee~2FztyFwzuslb-fXtqZbccc1QnvdfqlSAfMoMB7FOVMPrAaohI590ZUket4ktFm3bV-3aD5BOIWlHYmF4icbwmYU4jYRIaDDbUw~NfG8ujkagux-v4RNL-UACW86xRQ9UzVe3duwawl7tFQm~iIh5Xaqaz-Czk3wMdC5kSw7WsZFn0CKBXxuZOU5idAATfvdob3jMropvfjyuZv-2KwP4x9cqoVMgbkLQch6F0UTEvQ__&amp;Key-Pair-Id=APKAJLOHF5GGSLRBV4ZA</t>
-  </si>
-  <si>
     <t>Introducción 
 a los 
 Patrones de Diseño</t>
@@ -492,6 +489,9 @@
   </si>
   <si>
     <t>Danilo, O., Patricia, N., &amp; Vinicio, M. (2022). Análisis comparativo de Patrones de Diseño de Software. Polo Del Conocimiento: Revista Científico - Profesional, 7(7), 2146–2165. https://dialnet.unirioja.es/descarga/articulo/9042927.pdf</t>
+  </si>
+  <si>
+    <t>https://www.academia.edu/download/60132311/Introduccion-a-los-patrones-de-diseno20190727-56910-x3jn57.pdf</t>
   </si>
 </sst>
 </file>
@@ -1157,9 +1157,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1205,7 +1205,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1219,10 +1219,10 @@
         <v>43722</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>128</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>129</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>12</v>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="J2" s="38"/>
     </row>
-    <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1264,7 +1264,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>8</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>42939</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>48</v>
@@ -1831,7 +1831,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:26" ht="150" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>22</v>
       </c>
@@ -1844,14 +1844,14 @@
       <c r="D23" s="8">
         <v>45607</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>96</v>
+      <c r="E23" s="39" t="s">
+        <v>130</v>
       </c>
       <c r="F23" s="55" t="s">
         <v>93</v>
       </c>
       <c r="G23" s="58" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H23" s="57">
         <v>16400</v>
@@ -1875,13 +1875,13 @@
         <v>45606</v>
       </c>
       <c r="E24" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="F24" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="F24" s="54" t="s">
+      <c r="G24" s="58" t="s">
         <v>99</v>
-      </c>
-      <c r="G24" s="58" t="s">
-        <v>100</v>
       </c>
       <c r="H24" s="57">
         <v>16400</v>
@@ -1904,13 +1904,13 @@
         <v>45607</v>
       </c>
       <c r="E25" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="54" t="s">
+        <v>98</v>
+      </c>
+      <c r="G25" s="58" t="s">
         <v>101</v>
-      </c>
-      <c r="F25" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="G25" s="58" t="s">
-        <v>102</v>
       </c>
       <c r="H25" s="57">
         <v>4830</v>
@@ -1934,19 +1934,19 @@
         <v>45608</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F26" s="54" t="s">
         <v>93</v>
       </c>
       <c r="G26" s="58" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" s="57">
         <v>199</v>
       </c>
       <c r="I26" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="30" x14ac:dyDescent="0.25">
@@ -1963,13 +1963,13 @@
         <v>45609</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F27" s="54" t="s">
         <v>93</v>
       </c>
       <c r="G27" s="58" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H27" s="57">
         <v>4830</v>
@@ -1983,7 +1983,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>83</v>
@@ -1992,13 +1992,13 @@
         <v>45608</v>
       </c>
       <c r="E28" s="26" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="54" t="s">
         <v>93</v>
       </c>
       <c r="G28" s="59" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H28" s="57">
         <v>298</v>
@@ -2012,22 +2012,22 @@
         <v>28</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>107</v>
-      </c>
-      <c r="C29" s="11" t="s">
-        <v>108</v>
       </c>
       <c r="D29" s="8">
         <v>45610</v>
       </c>
       <c r="E29" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F29" s="56" t="s">
         <v>117</v>
       </c>
-      <c r="F29" s="56" t="s">
+      <c r="G29" s="59" t="s">
         <v>118</v>
-      </c>
-      <c r="G29" s="59" t="s">
-        <v>119</v>
       </c>
       <c r="H29" s="57">
         <v>2170</v>
@@ -2041,22 +2041,22 @@
         <v>29</v>
       </c>
       <c r="B30" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>112</v>
       </c>
       <c r="D30" s="8">
         <v>45608</v>
       </c>
       <c r="E30" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="F30" s="56" t="s">
         <v>121</v>
       </c>
-      <c r="F30" s="56" t="s">
+      <c r="G30" s="58" t="s">
         <v>122</v>
-      </c>
-      <c r="G30" s="58" t="s">
-        <v>123</v>
       </c>
       <c r="H30" s="57">
         <v>2170</v>
@@ -2070,10 +2070,10 @@
         <v>30</v>
       </c>
       <c r="B31" s="25" t="s">
+        <v>114</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>115</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>116</v>
       </c>
       <c r="D31" s="8">
         <v>45607</v>
@@ -2082,10 +2082,10 @@
         <v>47</v>
       </c>
       <c r="F31" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="G31" s="60" t="s">
         <v>126</v>
-      </c>
-      <c r="G31" s="60" t="s">
-        <v>127</v>
       </c>
       <c r="H31" s="57">
         <v>283</v>
@@ -2099,10 +2099,10 @@
         <v>31</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" s="8">
         <v>45607</v>
@@ -2116,10 +2116,10 @@
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="24"/>
       <c r="B33" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>124</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>125</v>
       </c>
       <c r="D33" s="8">
         <v>45607</v>

</xml_diff>